<commit_message>
Test data excel sheet
</commit_message>
<xml_diff>
--- a/Test Data/TC_146_Verify_Battery_Standby_And_Battery_Alarm_Limits_On_Addition_Deletion_Of_Ethernet.xlsx
+++ b/Test Data/TC_146_Verify_Battery_Standby_And_Battery_Alarm_Limits_On_Addition_Deletion_Of_Ethernet.xlsx
@@ -133,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,14 +289,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,12 +597,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -614,10 +614,10 @@
       <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -732,12 +732,10 @@
         <v>19</v>
       </c>
       <c r="K8" s="10">
-        <f>F8+0.132</f>
-        <v>0.432</v>
-      </c>
-      <c r="L8" s="24">
-        <f>G8+0.21296</f>
-        <v>0.82496000000000003</v>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="L8" s="22">
+        <v>0.21296000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -772,12 +770,10 @@
         <v>26</v>
       </c>
       <c r="K9" s="19">
-        <f>F9+0.132</f>
-        <v>0.40800000000000003</v>
-      </c>
-      <c r="L9" s="24">
-        <f>G9+0.21296</f>
-        <v>0.63895999999999997</v>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0.21296000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>